<commit_message>
Added information download and fixed logbook
</commit_message>
<xml_diff>
--- a/app/www/project_logbook.xlsx
+++ b/app/www/project_logbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t xml:space="preserve">Enterprise2-2023-11-08.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">badger</t>
   </si>
 </sst>
 </file>
@@ -537,6 +543,70 @@
         <v>21</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
changes to save files
</commit_message>
<xml_diff>
--- a/app/www/project_logbook.xlsx
+++ b/app/www/project_logbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t xml:space="preserve">badger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final1-2023-12-11.csv</t>
   </si>
 </sst>
 </file>
@@ -607,6 +619,38 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>